<commit_message>
Corrected Excel BOM version (Anderson 1327 (Red) and 1327G6 (Black)
</commit_message>
<xml_diff>
--- a/Other Files/Pi-Go-BOM.xlsx
+++ b/Other Files/Pi-Go-BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="116">
   <si>
     <t>Qty</t>
   </si>
@@ -305,7 +305,10 @@
     <t>Heavy Duty Power Connectors PP15/45 HOUSING ONLY RED</t>
   </si>
   <si>
-    <t>879-1327 (Mouser)</t>
+    <t>1327-BK</t>
+  </si>
+  <si>
+    <t>879-1327-BK (Mouser)</t>
   </si>
   <si>
     <t>Ass'y with CN1</t>
@@ -320,7 +323,10 @@
     <t>Heavy Duty Power Connectors PP15/45 HOUSING ONLY BLACK </t>
   </si>
   <si>
-    <t>879-1327-BK (Mouser)</t>
+    <t>1327G6-BK</t>
+  </si>
+  <si>
+    <t>879-1327G6-BK (Mouser)</t>
   </si>
   <si>
     <t>Ass'y with CN2</t>
@@ -371,6 +377,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -392,6 +399,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -924,14 +932,14 @@
       <c r="E16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="3" t="n">
-        <v>1327</v>
+      <c r="F16" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>1</v>
@@ -942,25 +950,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>1</v>
@@ -971,22 +979,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>1</v>
@@ -997,22 +1005,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>1</v>
@@ -1020,7 +1028,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G21" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I21" s="0" t="n">
         <f aca="false">SUM(I2:I19)</f>

</xml_diff>